<commit_message>
Simple test on my new computer
</commit_message>
<xml_diff>
--- a/DepthCharges/Mines.xlsx
+++ b/DepthCharges/Mines.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Dropbox\GitHub\PowerQueryBitsAndPieces\DepthCharges\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\DepthCharges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A40D9A8-32E2-40B5-871E-5180764A0A0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11CC1DEB-5F3D-4A00-A698-332CB1E38B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OCR_Conversion" sheetId="1" r:id="rId1"/>
@@ -24,8 +24,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="113" r:id="rId5"/>
-    <pivotCache cacheId="114" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="1" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{FCE2AD5D-F65C-4FA6-A056-5C36A1767C68}">
@@ -336,13 +336,13 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Consolas"/>
+      <name val="Garamond"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Consolas"/>
+      <name val="Garamond"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -381,7 +381,7 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Consolas"/>
+      <name val="Garamond"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -389,7 +389,7 @@
       <i/>
       <sz val="10"/>
       <color theme="3"/>
-      <name val="Consolas"/>
+      <name val="Garamond"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -397,14 +397,14 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Consolas"/>
+      <name val="Garamond"/>
       <family val="3"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Consolas"/>
+      <name val="Garamond"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -418,7 +418,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Consolas"/>
+      <name val="Garamond"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -603,7 +603,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yy"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
@@ -898,8 +898,8 @@
       <xdr:rowOff>122464</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>709143</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>730914</xdr:colOff>
       <xdr:row>75</xdr:row>
       <xdr:rowOff>122464</xdr:rowOff>
     </xdr:to>
@@ -942,8 +942,8 @@
       <xdr:rowOff>40821</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>868285</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>182484</xdr:colOff>
       <xdr:row>135</xdr:row>
       <xdr:rowOff>96153</xdr:rowOff>
     </xdr:to>
@@ -991,8 +991,8 @@
       <xdr:rowOff>18000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>547466</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>439890</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>124914</xdr:rowOff>
     </xdr:to>
@@ -1240,7 +1240,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CD8246DA-424D-4069-BBB3-51BD5C2A03C8}" name="PivotTable3" cacheId="113" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CD8246DA-424D-4069-BBB3-51BD5C2A03C8}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B5:L76" firstHeaderRow="1" firstDataRow="3" firstDataCol="2"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" compact="0" allDrilled="1" showAll="0" dataSourceSort="1">
@@ -1631,7 +1631,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{91FE9397-D60B-472A-AFFC-7511A07243CF}" name="PivotTable4" cacheId="114" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{91FE9397-D60B-472A-AFFC-7511A07243CF}" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="O82:X91" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" allDrilled="1" outline="0" subtotalTop="0" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
@@ -1823,9 +1823,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Biegert">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Organic">
   <a:themeElements>
-    <a:clrScheme name="Biegert Custom 2">
+    <a:clrScheme name="Organic">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1833,49 +1833,109 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="323232"/>
+        <a:srgbClr val="212121"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="F2F2F2"/>
+        <a:srgbClr val="DADADA"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="AA530E"/>
+        <a:srgbClr val="83992A"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="DF8931"/>
+        <a:srgbClr val="3C9770"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="F5C16C"/>
+        <a:srgbClr val="44709D"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFEFE0"/>
+        <a:srgbClr val="A23C33"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="DCAEE8"/>
+        <a:srgbClr val="D97828"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="FFC5E6"/>
+        <a:srgbClr val="DEB340"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="6B9F25"/>
+        <a:srgbClr val="A8BF4D"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="00B0F0"/>
+        <a:srgbClr val="B4CA80"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Biegert Spreadsheet Font">
+    <a:fontScheme name="Organic">
       <a:majorFont>
-        <a:latin typeface="Consolas"/>
+        <a:latin typeface="Garamond" panose="02020404030301010803"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="돋움"/>
+        <a:font script="Hans" typeface="方正舒体"/>
+        <a:font script="Hant" typeface="微軟正黑體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Cordia New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Consolas"/>
+        <a:latin typeface="Garamond" panose="02020404030301010803"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐ明朝"/>
+        <a:font script="Hang" typeface="바탕"/>
+        <a:font script="Hans" typeface="方正舒体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Angsana New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Glossy">
+    <a:fmtScheme name="Organic">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1884,78 +1944,50 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="62000"/>
-                <a:satMod val="180000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="65000">
-              <a:schemeClr val="phClr">
-                <a:tint val="32000"/>
-                <a:satMod val="250000"/>
+                <a:tint val="60000"/>
+                <a:lumMod val="110000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="23000"/>
-                <a:satMod val="300000"/>
+                <a:tint val="82000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
+        <a:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+            <a:duotone>
               <a:schemeClr val="phClr">
-                <a:shade val="15000"/>
-                <a:satMod val="180000"/>
+                <a:shade val="74000"/>
+                <a:satMod val="130000"/>
+                <a:lumMod val="90000"/>
               </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:shade val="45000"/>
-                <a:satMod val="170000"/>
+                <a:tint val="94000"/>
+                <a:satMod val="120000"/>
+                <a:lumMod val="104000"/>
               </a:schemeClr>
-            </a:gs>
-            <a:gs pos="70000">
-              <a:schemeClr val="phClr">
-                <a:tint val="99000"/>
-                <a:shade val="65000"/>
-                <a:satMod val="155000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="95500"/>
-                <a:shade val="100000"/>
-                <a:satMod val="155000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
+            </a:duotone>
+          </a:blip>
+          <a:tile tx="0" ty="0" sx="100000" sy="100000" flip="none" algn="tl"/>
+        </a:blipFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:tint val="95000"/>
-              <a:shade val="95000"/>
-              <a:satMod val="120000"/>
-            </a:schemeClr>
+            <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="55000" cap="flat" cmpd="thickThin" algn="ctr">
+        <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:tint val="90000"/>
-              <a:satMod val="130000"/>
-            </a:schemeClr>
+            <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="50800" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1964,47 +1996,25 @@
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="50800" dist="38100" dir="5400000" rotWithShape="0">
+            <a:innerShdw blurRad="25400" dist="12700" dir="13500000">
               <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
+                <a:alpha val="45000"/>
               </a:srgbClr>
-            </a:outerShdw>
+            </a:innerShdw>
           </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="50800" dist="38100" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
+                <a:alpha val="60000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="63500" dist="38100" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="45000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="glow" dir="t">
-              <a:rot lat="0" lon="0" rev="6360000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d contourW="1000" prstMaterial="flat">
-            <a:bevelT w="95250" h="101600"/>
-            <a:contourClr>
-              <a:schemeClr val="phClr">
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:contourClr>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -2029,7 +2039,7 @@
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
           <a:stretch/>
         </a:blipFill>
       </a:bgFillStyleLst>
@@ -2055,10 +2065,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" customWidth="1"/>
-    <col min="2" max="2" width="50.88671875" customWidth="1"/>
-    <col min="3" max="9" width="10.44140625" customWidth="1"/>
-    <col min="10" max="10" width="11.44140625" customWidth="1"/>
+    <col min="1" max="1" width="10.25" customWidth="1"/>
+    <col min="2" max="2" width="50.75" customWidth="1"/>
+    <col min="3" max="9" width="10.25" customWidth="1"/>
+    <col min="10" max="10" width="11.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -4153,22 +4163,22 @@
       <selection activeCell="P101" sqref="P101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.44140625" defaultRowHeight="13.2" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.25" defaultRowHeight="13.2" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="19" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.75" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="3" max="3" width="17.625" customWidth="1"/>
+    <col min="4" max="7" width="17.125" customWidth="1"/>
+    <col min="8" max="8" width="22.25" customWidth="1"/>
+    <col min="9" max="10" width="12.5" customWidth="1"/>
+    <col min="11" max="11" width="17.75" customWidth="1"/>
+    <col min="12" max="12" width="13.125" customWidth="1"/>
+    <col min="15" max="15" width="16.25" customWidth="1"/>
+    <col min="16" max="19" width="17.125" customWidth="1"/>
+    <col min="20" max="20" width="22.25" customWidth="1"/>
+    <col min="21" max="22" width="12.5" customWidth="1"/>
+    <col min="23" max="23" width="17.75" customWidth="1"/>
+    <col min="24" max="24" width="13.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -7149,16 +7159,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1770403-5943-4397-A9E4-651F0B4CCADE}">
   <dimension ref="A1:D373"/>
   <sheetViews>
-    <sheetView showFormulas="1" workbookViewId="0">
-      <selection activeCell="F118" sqref="F118"/>
-    </sheetView>
+    <sheetView showFormulas="1" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.875" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="9.875" customWidth="1"/>
+    <col min="4" max="4" width="8.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -12396,15 +12404,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9569B9A0-E949-4F52-9027-900D1A3AC414}">
   <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="18"/>
-    <col min="2" max="2" width="11.109375" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="18"/>
+    <col min="1" max="1" width="9" style="18"/>
+    <col min="2" max="2" width="11" style="18" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>